<commit_message>
set cell value function is implemented in the excel handle class
</commit_message>
<xml_diff>
--- a/Automation/data/actiTimeUsers.xlsx
+++ b/Automation/data/actiTimeUsers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanda\Downloads\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>email</t>
   </si>
@@ -186,11 +186,18 @@
   <si>
     <t>manager19</t>
   </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -543,19 +550,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="29.5546875"/>
+    <col min="2" max="2" customWidth="true" width="17.21875"/>
+    <col min="3" max="3" customWidth="true" width="30.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
@@ -585,10 +592,10 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>5</v>
       </c>
     </row>
@@ -616,166 +623,166 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="12.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
+      <c r="A2" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>47</v>
       </c>
     </row>

</xml_diff>